<commit_message>
Mise à jour Points et améliorations
</commit_message>
<xml_diff>
--- a/PointsEtAmeliorations.xlsx
+++ b/PointsEtAmeliorations.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Améliorations définitives</t>
   </si>
@@ -76,12 +76,6 @@
   </si>
   <si>
     <t>Boss à 50 PV</t>
-  </si>
-  <si>
-    <t>Saut</t>
-  </si>
-  <si>
-    <t>Double saut (saut utilisable dans les airs une fois)</t>
   </si>
   <si>
     <t>Dash</t>
@@ -146,12 +140,21 @@
   <si>
     <t>Allonge mêlée x3</t>
   </si>
+  <si>
+    <t>Pour le LD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coût commun </t>
+  </si>
+  <si>
+    <t>en fonction du nombre d'amélirorations déjà achetées</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -173,12 +176,6 @@
       <name val="Arial"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
@@ -192,6 +189,18 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0070C0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -216,7 +225,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -228,7 +237,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -512,7 +522,7 @@
   <dimension ref="A1:U1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -564,9 +574,11 @@
       <c r="U1" s="3"/>
     </row>
     <row r="2" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="A2" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
       <c r="D2" s="5" t="s">
         <v>9</v>
       </c>
@@ -574,7 +586,7 @@
         <v>10</v>
       </c>
       <c r="G2" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2" s="6">
         <f>I17</f>
@@ -594,9 +606,11 @@
       </c>
     </row>
     <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>10</v>
-      </c>
+      <c r="A3" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
       <c r="D3" s="5" t="s">
         <v>11</v>
       </c>
@@ -604,7 +618,7 @@
         <v>15</v>
       </c>
       <c r="G3" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H3" s="6">
         <f t="shared" ref="H3:H11" si="0">H2*1.2</f>
@@ -624,8 +638,8 @@
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>12</v>
+      <c r="A4" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>13</v>
@@ -634,7 +648,7 @@
         <v>30</v>
       </c>
       <c r="G4" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H4" s="6">
         <f t="shared" si="0"/>
@@ -654,11 +668,11 @@
       </c>
     </row>
     <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>14</v>
+      <c r="A5" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="G5" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H5" s="6">
         <f t="shared" si="0"/>
@@ -679,7 +693,7 @@
     </row>
     <row r="6" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>16</v>
@@ -689,7 +703,7 @@
         <v>350</v>
       </c>
       <c r="G6" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H6" s="6">
         <f t="shared" si="0"/>
@@ -709,8 +723,8 @@
       </c>
     </row>
     <row r="7" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>17</v>
+      <c r="A7" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>18</v>
@@ -720,7 +734,7 @@
         <v>500</v>
       </c>
       <c r="G7" s="5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H7" s="6">
         <f t="shared" si="0"/>
@@ -740,9 +754,11 @@
       </c>
     </row>
     <row r="8" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="5"/>
+      <c r="A8" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="G8" s="5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H8" s="6">
         <f t="shared" si="0"/>
@@ -762,9 +778,11 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="5"/>
+      <c r="A9" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="G9" s="5">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H9" s="6">
         <f t="shared" si="0"/>
@@ -784,11 +802,11 @@
       </c>
     </row>
     <row r="10" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="8" t="s">
-        <v>19</v>
+      <c r="A10" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="G10" s="5">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H10" s="6">
         <f t="shared" si="0"/>
@@ -809,31 +827,17 @@
     </row>
     <row r="11" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G11" s="5">
-        <v>10</v>
-      </c>
-      <c r="H11" s="6">
-        <f t="shared" si="0"/>
-        <v>1805.9231231999993</v>
-      </c>
-      <c r="I11" s="7">
-        <f t="shared" si="1"/>
-        <v>9085.5387391999975</v>
-      </c>
-      <c r="J11" s="7">
-        <f>H11/I17</f>
-        <v>5.1597803519999976</v>
-      </c>
-      <c r="K11" s="7">
-        <f>I11/I17</f>
-        <v>25.958682111999995</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="G11" s="5"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
     </row>
     <row r="12" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>21</v>
+      <c r="A12" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="D12" s="5"/>
       <c r="G12" s="5"/>
@@ -841,24 +845,26 @@
       <c r="K12" s="7"/>
     </row>
     <row r="13" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
-        <v>22</v>
+      <c r="A13" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="D13" s="5"/>
       <c r="G13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H13" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="H13" s="6"/>
-      <c r="I13" s="10" t="s">
-        <v>38</v>
+      <c r="I13" s="9" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H14" s="6">
         <v>17</v>
@@ -870,10 +876,10 @@
     </row>
     <row r="15" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H15" s="6">
         <v>8</v>
@@ -884,11 +890,11 @@
       </c>
     </row>
     <row r="16" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>27</v>
+      <c r="A16" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H16" s="5">
         <v>2</v>
@@ -899,13 +905,10 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
-        <v>29</v>
-      </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H17" s="6">
         <f>SUM(H14,H15,H16)</f>
@@ -917,9 +920,6 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
-        <v>30</v>
-      </c>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
@@ -938,11 +938,11 @@
       <c r="I20" s="7"/>
     </row>
     <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="9" t="s">
-        <v>31</v>
+      <c r="A21" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G21" s="5"/>
       <c r="H21" s="7"/>
@@ -950,7 +950,7 @@
     </row>
     <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G22" s="5"/>
       <c r="H22" s="7"/>
@@ -958,7 +958,7 @@
     </row>
     <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B23">
         <f>I17*2</f>
@@ -969,7 +969,7 @@
     </row>
     <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B24">
         <f>I17*2</f>
@@ -980,14 +980,14 @@
     </row>
     <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
     </row>
     <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B26">
         <f>I17*7</f>
@@ -997,8 +997,8 @@
       <c r="I26" s="7"/>
     </row>
     <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="11" t="s">
-        <v>41</v>
+      <c r="A27" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="B27">
         <f>I17*7</f>

</xml_diff>

<commit_message>
Mise à jour des prix et du GDD pour les PV des ennemis
</commit_message>
<xml_diff>
--- a/PointsEtAmeliorations.xlsx
+++ b/PointsEtAmeliorations.xlsx
@@ -99,9 +99,6 @@
     <t>Vitesse d'attaque</t>
   </si>
   <si>
-    <t>Ennemis à 3PV</t>
-  </si>
-  <si>
     <t>Cadence de tir à distance x1.5</t>
   </si>
   <si>
@@ -148,6 +145,9 @@
   </si>
   <si>
     <t>en fonction du nombre d'amélirorations déjà achetées</t>
+  </si>
+  <si>
+    <t>Ennemis à 3 PV</t>
   </si>
 </sst>
 </file>
@@ -522,7 +522,7 @@
   <dimension ref="A1:U1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -575,7 +575,7 @@
     </row>
     <row r="2" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -590,11 +590,11 @@
       </c>
       <c r="H2" s="6">
         <f>I17</f>
-        <v>350</v>
+        <v>160</v>
       </c>
       <c r="I2" s="7">
         <f>H2</f>
-        <v>350</v>
+        <v>160</v>
       </c>
       <c r="J2" s="7">
         <f>H2/I17</f>
@@ -607,7 +607,7 @@
     </row>
     <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
@@ -621,12 +621,12 @@
         <v>1</v>
       </c>
       <c r="H3" s="6">
-        <f t="shared" ref="H3:H11" si="0">H2*1.2</f>
-        <v>420</v>
+        <f t="shared" ref="H3:H10" si="0">H2*1.2</f>
+        <v>192</v>
       </c>
       <c r="I3" s="7">
-        <f t="shared" ref="I3:I11" si="1">I2+H3</f>
-        <v>770</v>
+        <f t="shared" ref="I3:I10" si="1">I2+H3</f>
+        <v>352</v>
       </c>
       <c r="J3" s="7">
         <f>H3/I17</f>
@@ -652,11 +652,11 @@
       </c>
       <c r="H4" s="6">
         <f t="shared" si="0"/>
-        <v>504</v>
+        <v>230.39999999999998</v>
       </c>
       <c r="I4" s="7">
         <f t="shared" si="1"/>
-        <v>1274</v>
+        <v>582.4</v>
       </c>
       <c r="J4" s="7">
         <f>H4/I17</f>
@@ -664,7 +664,7 @@
       </c>
       <c r="K4" s="7">
         <f>I4/I17</f>
-        <v>3.64</v>
+        <v>3.6399999999999997</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -676,15 +676,15 @@
       </c>
       <c r="H5" s="6">
         <f t="shared" si="0"/>
-        <v>604.79999999999995</v>
+        <v>276.47999999999996</v>
       </c>
       <c r="I5" s="7">
         <f t="shared" si="1"/>
-        <v>1878.8</v>
+        <v>858.87999999999988</v>
       </c>
       <c r="J5" s="7">
         <f>H5/I17</f>
-        <v>1.728</v>
+        <v>1.7279999999999998</v>
       </c>
       <c r="K5" s="7">
         <f>I5/I17</f>
@@ -707,19 +707,19 @@
       </c>
       <c r="H6" s="6">
         <f t="shared" si="0"/>
-        <v>725.75999999999988</v>
+        <v>331.77599999999995</v>
       </c>
       <c r="I6" s="7">
         <f t="shared" si="1"/>
-        <v>2604.56</v>
+        <v>1190.6559999999999</v>
       </c>
       <c r="J6" s="7">
         <f>H6/I17</f>
-        <v>2.0735999999999994</v>
+        <v>2.0735999999999999</v>
       </c>
       <c r="K6" s="7">
         <f>I6/I17</f>
-        <v>7.4416000000000002</v>
+        <v>7.4415999999999993</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -738,11 +738,11 @@
       </c>
       <c r="H7" s="6">
         <f t="shared" si="0"/>
-        <v>870.91199999999981</v>
+        <v>398.13119999999992</v>
       </c>
       <c r="I7" s="7">
         <f t="shared" si="1"/>
-        <v>3475.4719999999998</v>
+        <v>1588.7871999999998</v>
       </c>
       <c r="J7" s="7">
         <f>H7/I17</f>
@@ -762,11 +762,11 @@
       </c>
       <c r="H8" s="6">
         <f t="shared" si="0"/>
-        <v>1045.0943999999997</v>
+        <v>477.75743999999986</v>
       </c>
       <c r="I8" s="7">
         <f t="shared" si="1"/>
-        <v>4520.5663999999997</v>
+        <v>2066.5446399999996</v>
       </c>
       <c r="J8" s="7">
         <f>H8/I17</f>
@@ -774,7 +774,7 @@
       </c>
       <c r="K8" s="7">
         <f>I8/I17</f>
-        <v>12.915903999999999</v>
+        <v>12.915903999999998</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -786,11 +786,11 @@
       </c>
       <c r="H9" s="6">
         <f t="shared" si="0"/>
-        <v>1254.1132799999996</v>
+        <v>573.30892799999981</v>
       </c>
       <c r="I9" s="7">
         <f t="shared" si="1"/>
-        <v>5774.6796799999993</v>
+        <v>2639.8535679999995</v>
       </c>
       <c r="J9" s="7">
         <f>H9/I17</f>
@@ -810,11 +810,11 @@
       </c>
       <c r="H10" s="6">
         <f t="shared" si="0"/>
-        <v>1504.9359359999994</v>
+        <v>687.97071359999973</v>
       </c>
       <c r="I10" s="7">
         <f t="shared" si="1"/>
-        <v>7279.6156159999991</v>
+        <v>3327.8242815999993</v>
       </c>
       <c r="J10" s="7">
         <f>H10/I17</f>
@@ -827,7 +827,7 @@
     </row>
     <row r="11" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="6"/>
@@ -837,7 +837,7 @@
     </row>
     <row r="12" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D12" s="5"/>
       <c r="G12" s="5"/>
@@ -850,13 +850,13 @@
       </c>
       <c r="D13" s="5"/>
       <c r="G13" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -867,11 +867,11 @@
         <v>22</v>
       </c>
       <c r="H14" s="6">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="I14">
         <f>H14*10</f>
-        <v>170</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -882,11 +882,11 @@
         <v>24</v>
       </c>
       <c r="H15" s="6">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I15">
         <f>H15*15</f>
-        <v>120</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -894,29 +894,29 @@
         <v>23</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="H16" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I16">
         <f>H16*30</f>
-        <v>60</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H17" s="6">
         <f>SUM(H14,H15,H16)</f>
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="I17" s="6">
         <f>SUM(I14:I16)</f>
-        <v>350</v>
+        <v>160</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -939,10 +939,10 @@
     </row>
     <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>30</v>
       </c>
       <c r="G21" s="5"/>
       <c r="H21" s="7"/>
@@ -950,7 +950,7 @@
     </row>
     <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G22" s="5"/>
       <c r="H22" s="7"/>
@@ -958,51 +958,51 @@
     </row>
     <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23">
         <f>I17*2</f>
-        <v>700</v>
+        <v>320</v>
       </c>
       <c r="H23" s="7"/>
       <c r="I23" s="7"/>
     </row>
     <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24">
         <f>I17*2</f>
-        <v>700</v>
+        <v>320</v>
       </c>
       <c r="H24" s="7"/>
       <c r="I24" s="7"/>
     </row>
     <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
     </row>
     <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B26">
-        <f>I17*7</f>
-        <v>2450</v>
+        <f>I17*5</f>
+        <v>800</v>
       </c>
       <c r="H26" s="7"/>
       <c r="I26" s="7"/>
     </row>
     <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B27">
-        <f>I17*7</f>
-        <v>2450</v>
+        <f>I17*5</f>
+        <v>800</v>
       </c>
       <c r="H27" s="7"/>
       <c r="I27" s="7"/>

</xml_diff>